<commit_message>
recursos links con titulo, importacion
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/06_formato_cargue_links.xlsx
+++ b/assets/formatos_cargue/06_formato_cargue_links.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ele4\assets\formatos_cargue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ele\assets\formatos_cargue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Cód. tema</t>
   </si>
@@ -42,10 +42,25 @@
     <t>http://cienciasnaturalesyexperimentales.mex.tl/787887_CARACTER-STICAS-DE-LOS-SERES-VIVOS.html</t>
   </si>
   <si>
-    <t>m2-023</t>
-  </si>
-  <si>
-    <t>m2-031</t>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>titulo 1</t>
+  </si>
+  <si>
+    <t>titulo 2</t>
+  </si>
+  <si>
+    <t>titulo 3</t>
+  </si>
+  <si>
+    <t>titulo nuevo</t>
+  </si>
+  <si>
+    <t>ciencias naturales</t>
+  </si>
+  <si>
+    <t>l1-u01</t>
   </si>
 </sst>
 </file>
@@ -419,85 +434,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="94" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="94" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="29.5703125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
ImportacÃiÃon de links con archivo excel
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/06_formato_cargue_links.xlsx
+++ b/assets/formatos_cargue/06_formato_cargue_links.xlsx
@@ -13,54 +13,106 @@
   </bookViews>
   <sheets>
     <sheet name="links" sheetId="1" r:id="rId1"/>
+    <sheet name="referencia" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Cód. tema</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>http://alimentosconstructores123.blogspot.com/</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/iAU4-_YPq_w?rel=0</t>
-  </si>
-  <si>
-    <t>http://comidassaludables.info/alimentos-reguladores/</t>
-  </si>
-  <si>
-    <t>http://mara-animalesvertebrados.blogspot.com/</t>
-  </si>
-  <si>
-    <t>http://cienciasnaturalesyexperimentales.mex.tl/787887_CARACTER-STICAS-DE-LOS-SERES-VIVOS.html</t>
-  </si>
-  <si>
     <t>titulo</t>
   </si>
   <si>
-    <t>titulo 1</t>
-  </si>
-  <si>
-    <t>titulo 2</t>
-  </si>
-  <si>
-    <t>titulo 3</t>
-  </si>
-  <si>
-    <t>titulo nuevo</t>
-  </si>
-  <si>
-    <t>ciencias naturales</t>
-  </si>
-  <si>
-    <t>l1-u01</t>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>descripción</t>
+  </si>
+  <si>
+    <t>palabras clave</t>
+  </si>
+  <si>
+    <t>componente</t>
+  </si>
+  <si>
+    <t>ID componente</t>
+  </si>
+  <si>
+    <t>Aleatorio</t>
+  </si>
+  <si>
+    <t>Ciencia Tecnología y sociedad CTS</t>
+  </si>
+  <si>
+    <t>Relaciones espaciales y ambientales</t>
+  </si>
+  <si>
+    <t>Relaciones ético - políticas</t>
+  </si>
+  <si>
+    <t>Relaciones con la historia y las culturas</t>
+  </si>
+  <si>
+    <t>Entorno físico</t>
+  </si>
+  <si>
+    <t>Entorno vivo</t>
+  </si>
+  <si>
+    <t>Geométrico métrico</t>
+  </si>
+  <si>
+    <t>Numérico variacional</t>
+  </si>
+  <si>
+    <t>Pragmática</t>
+  </si>
+  <si>
+    <t>Semántico</t>
+  </si>
+  <si>
+    <t>Sintáctico</t>
+  </si>
+  <si>
+    <t>Argumentación</t>
+  </si>
+  <si>
+    <t>Conocimiento</t>
+  </si>
+  <si>
+    <t>Multiperspectividad</t>
+  </si>
+  <si>
+    <t>Pensamiento Sistémico</t>
+  </si>
+  <si>
+    <t>Comprensión e interpretación textual - Producción textual</t>
+  </si>
+  <si>
+    <t>Literatura</t>
+  </si>
+  <si>
+    <t>Medios de comunicación y otros sistemas simbólicos</t>
+  </si>
+  <si>
+    <t>La encuesta</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com</t>
+  </si>
+  <si>
+    <t>descripción de prueba, link importado</t>
+  </si>
+  <si>
+    <t>link prueba, ensayo, práctica, test</t>
+  </si>
+  <si>
+    <t>m5-082</t>
   </si>
 </sst>
 </file>
@@ -92,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +154,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +193,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -434,21 +510,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="94" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="79.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="29.5703125" style="3" customWidth="1"/>
@@ -460,14 +537,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -475,58 +558,26 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -535,4 +586,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="8">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="8">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="8">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="8">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="8">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="8">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="8">
+        <v>996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>